<commit_message>
chore: erase semester_aktif on create and export
</commit_message>
<xml_diff>
--- a/public/excel/template_semester.xlsx
+++ b/public/excel/template_semester.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
     <t>Nama Semester</t>
   </si>
@@ -26,16 +26,10 @@
     <t>Jenis (Ganjil/Genap)</t>
   </si>
   <si>
-    <t>Aktif (true/false)</t>
-  </si>
-  <si>
     <t>Semester Ganjil 2023</t>
   </si>
   <si>
     <t>Ganjil</t>
-  </si>
-  <si>
-    <t>true</t>
   </si>
 </sst>
 </file>
@@ -402,7 +396,7 @@
     <col min="1" max="1" width="24.708" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="6.998" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="24.708" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="22.28" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="9.10" bestFit="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -415,36 +409,22 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>2023</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>